<commit_message>
Pushed the excel and JUnit tests for Lab03
</commit_message>
<xml_diff>
--- a/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
+++ b/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28830"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B38A752F-EB82-4F2F-8876-C3E16DF5CDFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F21E759D-91B2-4CFB-B6DF-A86892431F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -307,7 +307,7 @@
     <t>F02_TC03</t>
   </si>
   <si>
-    <t>tasks = [task activ, nerepetitiv cu start=05/05/2025 10:00], start = 03/05/2025 10:00, end = 04/05/2025 10:00</t>
+    <t>tasks = [task activ, nerepetitiv cu start=05/05/2025 10:00], start = 06/05/2025 10:00, end = 07/05/2025 10:00</t>
   </si>
   <si>
     <t>1, 2, 3, 4, 5, 8</t>
@@ -2669,7 +2669,7 @@
   </sheetPr>
   <dimension ref="B1:AC16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -3278,8 +3278,8 @@
   </sheetPr>
   <dimension ref="B1:X12"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -3443,10 +3443,10 @@
         <v>112</v>
       </c>
       <c r="F8" s="38">
-        <v>45752.916666666664</v>
+        <v>45813.916666666664</v>
       </c>
       <c r="G8" s="38">
-        <v>45782.916666666664</v>
+        <v>45843.916666666664</v>
       </c>
       <c r="H8" s="37" t="s">
         <v>77</v>

</xml_diff>